<commit_message>
Mise à jour du fichier Fonctionnalite.xlsx
</commit_message>
<xml_diff>
--- a/Fonctionnalite.xlsx
+++ b/Fonctionnalite.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\33667\Documents\AI13\Projet\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\33667\Documents\AI13\Projet\GIT\ai13-projet-questionnaire\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{981E152F-5711-4D40-87AA-0BD7FD436E8D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A7F6BE93-9536-4D54-B718-923238548615}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{41DBFEBF-67B7-4A7D-879F-9DE653690FBA}"/>
   </bookViews>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="150" uniqueCount="84">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="162" uniqueCount="89">
   <si>
     <t>Fonctionalités</t>
   </si>
@@ -279,6 +279,21 @@
   </si>
   <si>
     <t xml:space="preserve"> login/mot de passe temporaire reçu par l'utilisateur</t>
+  </si>
+  <si>
+    <t>Qui</t>
+  </si>
+  <si>
+    <t>Jana</t>
+  </si>
+  <si>
+    <t>Imene</t>
+  </si>
+  <si>
+    <t>Jules</t>
+  </si>
+  <si>
+    <t>Jana (à la fin)</t>
   </si>
 </sst>
 </file>
@@ -339,7 +354,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="6">
+  <borders count="8">
     <border>
       <left/>
       <right/>
@@ -404,12 +419,36 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
@@ -426,6 +465,12 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="5" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -435,10 +480,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="5" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -446,21 +491,40 @@
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Titre 1" xfId="1" builtinId="16"/>
   </cellStyles>
-  <dxfs count="11">
+  <dxfs count="14">
     <dxf>
       <font>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="10"/>
-        <color theme="0"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
+        <sz val="9"/>
       </font>
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right/>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9"/>
+        </patternFill>
+      </fill>
     </dxf>
     <dxf>
       <fill>
@@ -572,6 +636,21 @@
     <dxf>
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <color theme="0"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
@@ -586,14 +665,15 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{E8AC9B7D-A3F4-45BE-9D93-0D1C2FAFEB98}" name="Tableau2" displayName="Tableau2" ref="A2:E37" totalsRowShown="0" headerRowDxfId="0" dataDxfId="10" tableBorderDxfId="9">
-  <autoFilter ref="A2:E37" xr:uid="{E8AC9B7D-A3F4-45BE-9D93-0D1C2FAFEB98}"/>
-  <tableColumns count="5">
-    <tableColumn id="1" xr3:uid="{478AB87D-2535-4291-9154-D88B9647B86F}" name="Type" dataDxfId="8"/>
-    <tableColumn id="2" xr3:uid="{4BC67698-DF41-4B2E-9AB7-DA4D116F320B}" name="Fonctionalités" dataDxfId="7"/>
-    <tableColumn id="3" xr3:uid="{83D53CE2-30D1-4C3A-923C-D8A0290ADC14}" name="Détail" dataDxfId="6"/>
-    <tableColumn id="4" xr3:uid="{7135C062-B069-4A83-AAEC-6D5E0948ECDB}" name="Fait (O/N)" dataDxfId="5"/>
-    <tableColumn id="5" xr3:uid="{688E299E-8E7F-4DE9-B854-79487FE92FE3}" name="Manque" dataDxfId="4"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{E8AC9B7D-A3F4-45BE-9D93-0D1C2FAFEB98}" name="Tableau2" displayName="Tableau2" ref="A2:F41" totalsRowShown="0" headerRowDxfId="13" dataDxfId="12" tableBorderDxfId="11">
+  <autoFilter ref="A2:F41" xr:uid="{E8AC9B7D-A3F4-45BE-9D93-0D1C2FAFEB98}"/>
+  <tableColumns count="6">
+    <tableColumn id="1" xr3:uid="{478AB87D-2535-4291-9154-D88B9647B86F}" name="Type" dataDxfId="10"/>
+    <tableColumn id="2" xr3:uid="{4BC67698-DF41-4B2E-9AB7-DA4D116F320B}" name="Fonctionalités" dataDxfId="9"/>
+    <tableColumn id="3" xr3:uid="{83D53CE2-30D1-4C3A-923C-D8A0290ADC14}" name="Détail" dataDxfId="8"/>
+    <tableColumn id="4" xr3:uid="{7135C062-B069-4A83-AAEC-6D5E0948ECDB}" name="Fait (O/N)" dataDxfId="7"/>
+    <tableColumn id="5" xr3:uid="{688E299E-8E7F-4DE9-B854-79487FE92FE3}" name="Manque" dataDxfId="6"/>
+    <tableColumn id="6" xr3:uid="{E9559D6E-9382-4200-B248-3B42C7D2B501}" name="Qui" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -896,10 +976,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CCB04502-5B20-4C26-992B-49C1A6028A39}">
-  <dimension ref="A1:E44"/>
+  <dimension ref="A1:F43"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A5" zoomScale="112" zoomScaleNormal="45" workbookViewId="0">
-      <selection activeCell="D10" sqref="D10"/>
+    <sheetView tabSelected="1" topLeftCell="A19" zoomScale="112" zoomScaleNormal="45" workbookViewId="0">
+      <selection activeCell="F29" sqref="F29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -908,35 +988,39 @@
     <col min="3" max="3" width="57.1796875" style="1" customWidth="1"/>
     <col min="4" max="4" width="13" style="2" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="16.36328125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="10.90625" style="4"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A1" s="6" t="s">
+    <row r="1" spans="1:6" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="A1" s="8" t="s">
         <v>46</v>
       </c>
-      <c r="B1" s="6"/>
-      <c r="C1" s="6"/>
-      <c r="D1" s="6"/>
-      <c r="E1" s="6"/>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A2" s="9" t="s">
+      <c r="B1" s="8"/>
+      <c r="C1" s="8"/>
+      <c r="D1" s="8"/>
+      <c r="E1" s="8"/>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A2" s="6" t="s">
         <v>51</v>
       </c>
-      <c r="B2" s="9" t="s">
+      <c r="B2" s="6" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="10" t="s">
+      <c r="C2" s="7" t="s">
         <v>3</v>
       </c>
-      <c r="D2" s="10" t="s">
+      <c r="D2" s="7" t="s">
         <v>72</v>
       </c>
-      <c r="E2" s="10" t="s">
+      <c r="E2" s="7" t="s">
         <v>71</v>
       </c>
-    </row>
-    <row r="3" spans="1:5" ht="28.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="F2" s="4" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" ht="28.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A3" s="3" t="s">
         <v>52</v>
       </c>
@@ -951,7 +1035,7 @@
       </c>
       <c r="E3" s="4"/>
     </row>
-    <row r="4" spans="1:5" ht="29.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:6" ht="29.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A4" s="3" t="s">
         <v>52</v>
       </c>
@@ -966,7 +1050,7 @@
       </c>
       <c r="E4" s="4"/>
     </row>
-    <row r="5" spans="1:5" ht="19.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:6" ht="19.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A5" s="3" t="s">
         <v>53</v>
       </c>
@@ -981,7 +1065,7 @@
       </c>
       <c r="E5" s="4"/>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A6" s="3" t="s">
         <v>52</v>
       </c>
@@ -994,7 +1078,7 @@
       </c>
       <c r="E6" s="4"/>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A7" s="3" t="s">
         <v>52</v>
       </c>
@@ -1007,7 +1091,7 @@
       </c>
       <c r="E7" s="4"/>
     </row>
-    <row r="8" spans="1:5" ht="24" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:6" ht="24" x14ac:dyDescent="0.35">
       <c r="A8" s="3" t="s">
         <v>52</v>
       </c>
@@ -1018,11 +1102,11 @@
         <v>78</v>
       </c>
       <c r="D8" s="4" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="E8" s="4"/>
     </row>
-    <row r="9" spans="1:5" ht="24" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:6" ht="24" x14ac:dyDescent="0.35">
       <c r="A9" s="3" t="s">
         <v>52</v>
       </c>
@@ -1035,7 +1119,7 @@
       </c>
       <c r="E9" s="4"/>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A10" s="3" t="s">
         <v>52</v>
       </c>
@@ -1051,8 +1135,11 @@
       <c r="E10" s="4" t="s">
         <v>75</v>
       </c>
-    </row>
-    <row r="11" spans="1:5" ht="33" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="F10" s="4" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" ht="33" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A11" s="3" t="s">
         <v>52</v>
       </c>
@@ -1067,7 +1154,7 @@
       </c>
       <c r="E11" s="4"/>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A12" s="3" t="s">
         <v>52</v>
       </c>
@@ -1081,8 +1168,11 @@
         <v>74</v>
       </c>
       <c r="E12" s="4"/>
-    </row>
-    <row r="13" spans="1:5" ht="23" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="F12" s="4" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" ht="23" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A13" s="3" t="s">
         <v>52</v>
       </c>
@@ -1096,8 +1186,11 @@
         <v>74</v>
       </c>
       <c r="E13" s="4"/>
-    </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F13" s="4" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A14" s="3" t="s">
         <v>52</v>
       </c>
@@ -1111,8 +1204,11 @@
         <v>74</v>
       </c>
       <c r="E14" s="4"/>
-    </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F14" s="4" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A15" s="3" t="s">
         <v>52</v>
       </c>
@@ -1127,7 +1223,7 @@
       </c>
       <c r="E15" s="4"/>
     </row>
-    <row r="16" spans="1:5" ht="32.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:6" ht="32.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A16" s="3" t="s">
         <v>52</v>
       </c>
@@ -1143,8 +1239,11 @@
       <c r="E16" s="4" t="s">
         <v>76</v>
       </c>
-    </row>
-    <row r="17" spans="1:5" ht="32.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="F16" s="4" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" ht="32.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A17" s="3" t="s">
         <v>52</v>
       </c>
@@ -1160,8 +1259,11 @@
       <c r="E17" s="4" t="s">
         <v>76</v>
       </c>
-    </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F17" s="4" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A18" s="3" t="s">
         <v>68</v>
       </c>
@@ -1175,8 +1277,11 @@
         <v>74</v>
       </c>
       <c r="E18" s="4"/>
-    </row>
-    <row r="19" spans="1:5" ht="28.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="F18" s="4" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" ht="28.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A19" s="3" t="s">
         <v>68</v>
       </c>
@@ -1193,7 +1298,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A20" s="3" t="s">
         <v>68</v>
       </c>
@@ -1208,7 +1313,7 @@
       </c>
       <c r="E20" s="4"/>
     </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A21" s="3" t="s">
         <v>68</v>
       </c>
@@ -1225,7 +1330,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A22" s="3" t="s">
         <v>68</v>
       </c>
@@ -1242,7 +1347,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="23" spans="1:5" ht="24" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:6" ht="24" x14ac:dyDescent="0.35">
       <c r="A23" s="3" t="s">
         <v>68</v>
       </c>
@@ -1259,7 +1364,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="24" spans="1:5" ht="24" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:6" ht="24" x14ac:dyDescent="0.35">
       <c r="A24" s="3" t="s">
         <v>53</v>
       </c>
@@ -1273,8 +1378,11 @@
         <v>74</v>
       </c>
       <c r="E24" s="4"/>
-    </row>
-    <row r="25" spans="1:5" ht="24" x14ac:dyDescent="0.35">
+      <c r="F24" s="4" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" ht="24" x14ac:dyDescent="0.35">
       <c r="A25" s="3" t="s">
         <v>68</v>
       </c>
@@ -1291,7 +1399,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A26" s="3" t="s">
         <v>68</v>
       </c>
@@ -1305,8 +1413,11 @@
         <v>74</v>
       </c>
       <c r="E26" s="4"/>
-    </row>
-    <row r="27" spans="1:5" ht="24" x14ac:dyDescent="0.35">
+      <c r="F26" s="4" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6" ht="24" x14ac:dyDescent="0.35">
       <c r="A27" s="3"/>
       <c r="B27" s="3" t="s">
         <v>27</v>
@@ -1318,8 +1429,11 @@
         <v>74</v>
       </c>
       <c r="E27" s="4"/>
-    </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F27" s="4" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A28" s="3"/>
       <c r="B28" s="5" t="s">
         <v>44</v>
@@ -1331,8 +1445,11 @@
         <v>74</v>
       </c>
       <c r="E28" s="4"/>
-    </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F28" s="4" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A29" s="3" t="s">
         <v>69</v>
       </c>
@@ -1347,7 +1464,7 @@
       </c>
       <c r="E29" s="4"/>
     </row>
-    <row r="30" spans="1:5" ht="24" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:6" ht="24" x14ac:dyDescent="0.35">
       <c r="A30" s="3" t="s">
         <v>69</v>
       </c>
@@ -1362,7 +1479,7 @@
       </c>
       <c r="E30" s="4"/>
     </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A31" s="3" t="s">
         <v>70</v>
       </c>
@@ -1377,7 +1494,7 @@
       </c>
       <c r="E31" s="4"/>
     </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A32" s="3" t="s">
         <v>69</v>
       </c>
@@ -1466,34 +1583,52 @@
       <c r="E37" s="4"/>
     </row>
     <row r="38" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="D38"/>
+      <c r="A38" s="3"/>
+      <c r="B38" s="3"/>
+      <c r="C38" s="3"/>
+      <c r="D38" s="4"/>
+      <c r="E38" s="4"/>
     </row>
     <row r="39" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="D39"/>
+      <c r="A39" s="3"/>
+      <c r="B39" s="3"/>
+      <c r="C39" s="3"/>
+      <c r="D39" s="4"/>
+      <c r="E39" s="4"/>
     </row>
     <row r="40" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="D40"/>
+      <c r="A40" s="3"/>
+      <c r="B40" s="3"/>
+      <c r="C40" s="3"/>
+      <c r="D40" s="4"/>
+      <c r="E40" s="4"/>
     </row>
     <row r="41" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="D41"/>
+      <c r="A41" s="11"/>
+      <c r="B41" s="11"/>
+      <c r="C41" s="11"/>
+      <c r="D41" s="12"/>
+      <c r="E41" s="12"/>
     </row>
     <row r="42" spans="1:5" x14ac:dyDescent="0.35">
       <c r="D42"/>
     </row>
     <row r="43" spans="1:5" x14ac:dyDescent="0.35">
       <c r="D43"/>
-    </row>
-    <row r="44" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="D44"/>
     </row>
   </sheetData>
   <mergeCells count="1">
     <mergeCell ref="A1:E1"/>
   </mergeCells>
   <phoneticPr fontId="4" type="noConversion"/>
-  <conditionalFormatting sqref="A2:E37">
-    <cfRule type="expression" dxfId="1" priority="1">
+  <conditionalFormatting sqref="A2:E41">
+    <cfRule type="expression" dxfId="4" priority="3">
       <formula>$D2="O"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F1:F1048576">
+    <cfRule type="expression" dxfId="2" priority="1">
+      <formula>$D1="O"</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.25" right="0.25" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1515,11 +1650,11 @@
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>
     <row r="1" spans="1:3" ht="19.5" x14ac:dyDescent="0.45">
-      <c r="A1" s="7" t="s">
+      <c r="A1" s="9" t="s">
         <v>49</v>
       </c>
-      <c r="B1" s="7"/>
-      <c r="C1" s="7"/>
+      <c r="B1" s="9"/>
+      <c r="C1" s="9"/>
     </row>
   </sheetData>
   <mergeCells count="1">
@@ -1541,11 +1676,11 @@
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A1" s="8" t="s">
+      <c r="A1" s="10" t="s">
         <v>50</v>
       </c>
-      <c r="B1" s="8"/>
-      <c r="C1" s="8"/>
+      <c r="B1" s="10"/>
+      <c r="C1" s="10"/>
     </row>
   </sheetData>
   <mergeCells count="1">

</xml_diff>